<commit_message>
20220129T140100 - Nearest Neighbour implemented and complete. K-Nearest Neighbour implemented. Included statistics.
</commit_message>
<xml_diff>
--- a/logs/stats.xlsx
+++ b/logs/stats.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.camilleri\IdeaProjects\Test\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD128GB/Google Drive/Education/MDX BSc CS/Modules/7 - CST3170 - Artificial Intelligence/Courseworks/CW2/Test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9DBA05-F401-8746-A387-0373A79C03F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22680" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,11 +107,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,24 +395,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -449,8 +464,12 @@
         <f>ROUND(F2*100/E2,4)</f>
         <v>98.042699999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3">
+        <f>ROUND(AVERAGE(H2,H3),4)</f>
+        <v>98.256299999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -474,8 +493,9 @@
         <f t="shared" ref="H3:H17" si="1">ROUND(F3*100/E3,4)</f>
         <v>98.469800000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -502,8 +522,12 @@
         <f t="shared" si="1"/>
         <v>97.331000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3">
+        <f>ROUND(AVERAGE(H4,H5),4)</f>
+        <v>97.437799999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -530,8 +554,9 @@
         <f t="shared" si="1"/>
         <v>97.544499999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -558,8 +583,12 @@
         <f t="shared" si="1"/>
         <v>97.259799999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <f>ROUND(AVERAGE(H6,H7),4)</f>
+        <v>97.544499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -586,8 +615,9 @@
         <f t="shared" si="1"/>
         <v>97.8292</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -614,8 +644,12 @@
         <f t="shared" si="1"/>
         <v>97.615700000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <f>ROUND(AVERAGE(H8,H9),4)</f>
+        <v>97.758099999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -642,8 +676,9 @@
         <f t="shared" si="1"/>
         <v>97.900400000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -670,8 +705,12 @@
         <f t="shared" si="1"/>
         <v>97.757999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <f>ROUND(AVERAGE(H10,H11),4)</f>
+        <v>98.060500000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -698,8 +737,9 @@
         <f t="shared" si="1"/>
         <v>98.363</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -726,8 +766,12 @@
         <f t="shared" si="1"/>
         <v>97.864800000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <f>ROUND(AVERAGE(H12,H13),4)</f>
+        <v>97.953800000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -754,8 +798,9 @@
         <f t="shared" si="1"/>
         <v>98.042699999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -782,8 +827,12 @@
         <f t="shared" si="1"/>
         <v>98.078299999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="3">
+        <f>ROUND(AVERAGE(H14,H15),4)</f>
+        <v>98.096100000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -810,8 +859,9 @@
         <f t="shared" si="1"/>
         <v>98.113900000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -838,8 +888,12 @@
         <f t="shared" si="1"/>
         <v>97.0107</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="3">
+        <f>ROUND(AVERAGE(H16,H17),4)</f>
+        <v>97.331000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -866,8 +920,19 @@
         <f t="shared" si="1"/>
         <v>97.651200000000003</v>
       </c>
+      <c r="I17" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
20220202T010300 - Nearest Neighbour implemented and complete. K-Nearest Neighbour implemented and complete. Included statistics. TODO: Continue working on K-Means -> check means calculation and apply NN.
</commit_message>
<xml_diff>
--- a/logs/stats.xlsx
+++ b/logs/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD128GB/Google Drive/Education/MDX BSc CS/Modules/7 - CST3170 - Artificial Intelligence/Courseworks/CW2/Test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9DBA05-F401-8746-A387-0373A79C03F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEE544-948C-FE44-AFDF-14F543087F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22680" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>Algorithm</t>
   </si>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -486,11 +486,11 @@
         <v>2767</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G17" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G19" si="0">E3-F3</f>
         <v>43</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H17" si="1">ROUND(F3*100/E3,4)</f>
+        <f t="shared" ref="H3:H19" si="1">ROUND(F3*100/E3,4)</f>
         <v>98.469800000000006</v>
       </c>
       <c r="I3" s="3"/>
@@ -922,8 +922,70 @@
       </c>
       <c r="I17" s="3"/>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2810</v>
+      </c>
+      <c r="F18">
+        <v>2755</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>98.042699999999996</v>
+      </c>
+      <c r="I18" s="3">
+        <f>ROUND(AVERAGE(H18,H19),4)</f>
+        <v>98.256299999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2810</v>
+      </c>
+      <c r="F19">
+        <v>2767</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>98.469800000000006</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="I18:I19"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="I2:I3"/>

</xml_diff>

<commit_message>
20220209T014200 - Nearest Neighbour implemented and complete. K-Nearest Neighbour implemented and complete. K-Means (simplified) implemented and complete. K-Means2 implemented and complete. K-Medians under development. Included statistics.
</commit_message>
<xml_diff>
--- a/logs/stats.xlsx
+++ b/logs/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD128GB/Google Drive/Education/MDX BSc CS/Modules/7 - CST3170 - Artificial Intelligence/Courseworks/CW2/Test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD91184-0459-4C4D-B485-D6B7FD1D1206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B395F19-A521-6E4A-845E-C4B181DB1493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="-19640" windowWidth="22680" windowHeight="18340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="-19640" windowWidth="29400" windowHeight="18340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.000000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +106,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,10 +143,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -161,9 +170,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -199,12 +215,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -213,7 +226,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Best Results</a:t>
+              <a:t>Algorithm Comparison - best results </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -231,12 +244,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -274,9 +284,32 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -288,9 +321,32 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -303,7 +359,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -316,6 +372,61 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-MT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Aggregated!$E$2:$E$4</c:f>
@@ -337,16 +448,16 @@
             <c:numRef>
               <c:f>Aggregated!$F$2:$F$4</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000000%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>98.256227999999993</c:v>
+                  <c:v>0.9825622799999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.096086</c:v>
+                  <c:v>0.98096086000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.427046000000004</c:v>
+                  <c:v>0.90427046000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,15 +469,16 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="307465983"/>
         <c:axId val="204341855"/>
       </c:barChart>
@@ -385,7 +497,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="tx2">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -401,10 +513,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -432,7 +541,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -442,7 +551,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -460,10 +569,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -495,7 +601,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -537,6 +643,28 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm Comparison - averaged results</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -550,12 +678,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -593,9 +718,32 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -607,9 +755,32 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -622,7 +793,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -635,6 +806,60 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-MT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Aggregated!$E$8:$E$10</c:f>
@@ -656,16 +881,16 @@
             <c:numRef>
               <c:f>Aggregated!$F$8:$F$10</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000000%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>98.256227999999993</c:v>
+                  <c:v>0.9825622799999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.788849533333348</c:v>
+                  <c:v>0.97788849533333355</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.427046000000004</c:v>
+                  <c:v>0.90427046000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,15 +902,16 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="307760879"/>
         <c:axId val="307734463"/>
       </c:barChart>
@@ -704,7 +930,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="tx2">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -720,10 +946,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -751,7 +974,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -761,7 +984,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -779,10 +1002,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -814,7 +1034,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -856,6 +1076,28 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>K-Nearest Neighbour (two-fold)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -869,12 +1111,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -909,7 +1148,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -921,31 +1160,41 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="12700" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Aggregated!$B$45:$B$59</c:f>
@@ -1004,52 +1253,52 @@
             <c:numRef>
               <c:f>Aggregated!$C$45:$C$59</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>0.000000%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>97.437723000000005</c:v>
+                  <c:v>0.97437723000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.437723000000005</c:v>
+                  <c:v>0.97437723000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.633452000000005</c:v>
+                  <c:v>0.97633452000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.544483999999997</c:v>
+                  <c:v>0.97544483999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.633452000000005</c:v>
+                  <c:v>0.97633452000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.758007000000006</c:v>
+                  <c:v>0.97758007000000013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97.971530000000001</c:v>
+                  <c:v>0.97971530000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>97.846975</c:v>
+                  <c:v>0.97846975000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.971530999999999</c:v>
+                  <c:v>0.97971531000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97.900356000000002</c:v>
+                  <c:v>0.97900355999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98.060497999999995</c:v>
+                  <c:v>0.98060497999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.953737000000004</c:v>
+                  <c:v>0.97953737000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98.096086</c:v>
+                  <c:v>0.98096086000000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.330961000000002</c:v>
+                  <c:v>0.97330961000000005</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>98.256227999999993</c:v>
+                  <c:v>0.9825622799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1083,7 +1332,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1093,6 +1342,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>value of K</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-MT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1101,9 +1399,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1117,10 +1415,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1133,6 +1428,7 @@
         <c:crossAx val="307272383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="307272383"/>
@@ -1145,7 +1441,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1155,20 +1451,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1179,10 +1474,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1214,7 +1506,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1362,33 +1654,27 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1403,7 +1689,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1411,7 +1697,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1419,17 +1705,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -1438,9 +1721,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -1463,35 +1745,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1500,33 +1782,32 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1542,21 +1823,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1590,64 +1866,157 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1655,102 +2024,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1758,17 +2031,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -1777,12 +2050,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1791,14 +2061,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1807,10 +2077,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -1819,7 +2086,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1840,10 +2107,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -1852,46 +2116,34 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1906,7 +2158,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1914,7 +2166,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1922,17 +2174,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -1941,9 +2190,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -1966,35 +2214,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2003,33 +2251,32 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2045,21 +2292,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2093,64 +2335,157 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2158,102 +2493,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2261,17 +2500,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2280,12 +2519,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2294,14 +2530,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2310,10 +2546,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -2322,7 +2555,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2343,10 +2576,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -2355,48 +2585,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2409,7 +2627,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2417,7 +2635,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2425,17 +2643,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -2444,9 +2659,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -2469,35 +2683,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2509,18 +2723,19 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -2529,10 +2744,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2548,21 +2763,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2572,23 +2782,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2597,64 +2806,156 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2662,102 +2963,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2765,17 +2970,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2784,12 +2989,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2798,14 +3000,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2814,10 +3015,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -2826,20 +3024,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2848,20 +3045,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2871,14 +3064,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4352,17 +4539,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80050CAB-03EC-8548-BBAA-F2E0D74C6B64}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -4393,8 +4580,9 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7">
-        <v>98.256227999999993</v>
+      <c r="F2" s="10">
+        <f>98.256228*0.01</f>
+        <v>0.9825622799999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4410,8 +4598,9 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7">
-        <v>98.096086</v>
+      <c r="F3" s="10">
+        <f>98.096086*0.01</f>
+        <v>0.98096086000000005</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4427,8 +4616,9 @@
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7">
-        <v>90.427046000000004</v>
+      <c r="F4" s="10">
+        <f>90.427046*0.01</f>
+        <v>0.90427046000000011</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4483,8 +4673,9 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7">
-        <v>98.256227999999993</v>
+      <c r="F8" s="10">
+        <f>98.256228*0.01</f>
+        <v>0.9825622799999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4500,9 +4691,9 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7">
-        <f>AVERAGE(C3:C17)</f>
-        <v>97.788849533333348</v>
+      <c r="F9" s="10">
+        <f>AVERAGE(C3:C17)*0.01</f>
+        <v>0.97788849533333355</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4518,8 +4709,9 @@
       <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="7">
-        <v>90.427046000000004</v>
+      <c r="F10" s="10">
+        <f>90.427046*0.01</f>
+        <v>0.90427046000000011</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4632,8 +4824,8 @@
       <c r="B45" s="2">
         <v>15</v>
       </c>
-      <c r="C45" s="7">
-        <v>97.437723000000005</v>
+      <c r="C45" s="11">
+        <v>0.97437723000000009</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -4643,8 +4835,8 @@
       <c r="B46" s="2">
         <v>14</v>
       </c>
-      <c r="C46" s="7">
-        <v>97.437723000000005</v>
+      <c r="C46" s="11">
+        <v>0.97437723000000009</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -4654,8 +4846,8 @@
       <c r="B47" s="2">
         <v>13</v>
       </c>
-      <c r="C47" s="7">
-        <v>97.633452000000005</v>
+      <c r="C47" s="11">
+        <v>0.97633452000000009</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -4665,8 +4857,8 @@
       <c r="B48" s="2">
         <v>12</v>
       </c>
-      <c r="C48" s="7">
-        <v>97.544483999999997</v>
+      <c r="C48" s="11">
+        <v>0.97544483999999998</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -4676,8 +4868,8 @@
       <c r="B49" s="2">
         <v>11</v>
       </c>
-      <c r="C49" s="7">
-        <v>97.633452000000005</v>
+      <c r="C49" s="11">
+        <v>0.97633452000000009</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -4687,8 +4879,8 @@
       <c r="B50" s="2">
         <v>10</v>
       </c>
-      <c r="C50" s="7">
-        <v>97.758007000000006</v>
+      <c r="C50" s="11">
+        <v>0.97758007000000013</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -4698,8 +4890,8 @@
       <c r="B51" s="2">
         <v>9</v>
       </c>
-      <c r="C51" s="7">
-        <v>97.971530000000001</v>
+      <c r="C51" s="11">
+        <v>0.97971530000000007</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -4709,8 +4901,8 @@
       <c r="B52" s="2">
         <v>8</v>
       </c>
-      <c r="C52" s="7">
-        <v>97.846975</v>
+      <c r="C52" s="11">
+        <v>0.97846975000000003</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -4720,8 +4912,8 @@
       <c r="B53" s="2">
         <v>7</v>
       </c>
-      <c r="C53" s="7">
-        <v>97.971530999999999</v>
+      <c r="C53" s="11">
+        <v>0.97971531000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -4731,8 +4923,8 @@
       <c r="B54" s="2">
         <v>6</v>
       </c>
-      <c r="C54" s="7">
-        <v>97.900356000000002</v>
+      <c r="C54" s="11">
+        <v>0.97900355999999999</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -4742,8 +4934,8 @@
       <c r="B55" s="2">
         <v>5</v>
       </c>
-      <c r="C55" s="7">
-        <v>98.060497999999995</v>
+      <c r="C55" s="11">
+        <v>0.98060497999999996</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -4753,8 +4945,8 @@
       <c r="B56" s="2">
         <v>4</v>
       </c>
-      <c r="C56" s="7">
-        <v>97.953737000000004</v>
+      <c r="C56" s="11">
+        <v>0.97953737000000007</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -4764,8 +4956,8 @@
       <c r="B57" s="2">
         <v>3</v>
       </c>
-      <c r="C57" s="7">
-        <v>98.096086</v>
+      <c r="C57" s="11">
+        <v>0.98096086000000005</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -4775,8 +4967,8 @@
       <c r="B58" s="2">
         <v>2</v>
       </c>
-      <c r="C58" s="7">
-        <v>97.330961000000002</v>
+      <c r="C58" s="11">
+        <v>0.97330961000000005</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -4786,8 +4978,8 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="7">
-        <v>98.256227999999993</v>
+      <c r="C59" s="11">
+        <v>0.9825622799999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20220218T225700 - Nearest Neighbour implemented and complete. K-Nearest Neighbour implemented and complete. K-Means (simplified) implemented and complete. K-Means2 implemented and complete. K-Medians implemented and complete. Dataset shuffling implemented and complete. Included logs and statistics.
</commit_message>
<xml_diff>
--- a/logs/stats.xlsx
+++ b/logs/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD128GB/Google Drive/Education/MDX BSc CS/Modules/7 - CST3170 - Artificial Intelligence/Courseworks/CW2/Test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B395F19-A521-6E4A-845E-C4B181DB1493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF820873-DE44-B743-A54F-25608F529726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="-19640" windowWidth="29400" windowHeight="18340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="-20360" windowWidth="29400" windowHeight="18340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
   <si>
     <t>Algorithm</t>
   </si>
@@ -55,19 +55,10 @@
     <t>k Value</t>
   </si>
   <si>
-    <t>NN</t>
-  </si>
-  <si>
     <t>Successful Classifications</t>
   </si>
   <si>
-    <t>KNN</t>
-  </si>
-  <si>
     <t>Number of tests</t>
-  </si>
-  <si>
-    <t>KMeans</t>
   </si>
   <si>
     <t>Two-fold</t>
@@ -79,13 +70,19 @@
     <t>K-Nearest Neighbour</t>
   </si>
   <si>
-    <t>Simplified K-Means</t>
-  </si>
-  <si>
     <t>K-Nearest Neighbour (k==3)</t>
   </si>
   <si>
     <t>K-Nearest Neighbour (average)</t>
+  </si>
+  <si>
+    <t>Supervised K-Means</t>
+  </si>
+  <si>
+    <t>Supervised K-Means v2</t>
+  </si>
+  <si>
+    <t>Supervised K-Medians</t>
   </si>
 </sst>
 </file>
@@ -93,8 +90,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.000000%"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -153,28 +150,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -315,6 +312,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C853-F84E-A589-8F8FB20ED03E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -352,6 +354,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C853-F84E-A589-8F8FB20ED03E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -371,6 +378,80 @@
                 <c16:uniqueId val="{00000002-D38A-9E4D-9E93-3B16D157EAA1}"/>
               </c:ext>
             </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="0.00%" sourceLinked="0"/>
@@ -429,9 +510,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregated!$E$2:$E$4</c:f>
+              <c:f>Aggregated!$E$2:$E$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Nearest Neighbour</c:v>
                 </c:pt>
@@ -439,17 +520,23 @@
                   <c:v>K-Nearest Neighbour (k==3)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Simplified K-Means</c:v>
+                  <c:v>Supervised K-Means</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Supervised K-Means v2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Supervised K-Medians</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregated!$F$2:$F$4</c:f>
+              <c:f>Aggregated!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.9825622799999999</c:v>
                 </c:pt>
@@ -458,6 +545,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.90427046000000011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39003559000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89697508999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,7 +796,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aggregated!$F$7</c:f>
+              <c:f>Aggregated!$F$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -749,6 +842,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8E1C-A440-AADF-23717A4C8749}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -786,6 +884,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8E1C-A440-AADF-23717A4C8749}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -805,6 +908,80 @@
                 <c16:uniqueId val="{00000002-4338-CD4E-845A-F0ED836BBF7E}"/>
               </c:ext>
             </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -862,9 +1039,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregated!$E$8:$E$10</c:f>
+              <c:f>Aggregated!$E$10:$E$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Nearest Neighbour</c:v>
                 </c:pt>
@@ -872,17 +1049,23 @@
                   <c:v>K-Nearest Neighbour (average)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Simplified K-Means</c:v>
+                  <c:v>Supervised K-Means</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Supervised K-Means v2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Supervised K-Medians</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregated!$F$8:$F$10</c:f>
+              <c:f>Aggregated!$F$10:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000000%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.9825622799999999</c:v>
                 </c:pt>
@@ -891,6 +1074,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.90427046000000011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39003559000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89697508999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3080,8 +3269,8 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -3116,8 +3305,8 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3152,8 +3341,8 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3446,23 +3635,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3479,10 +3666,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -3491,14 +3678,14 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6"/>
+      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8"/>
       <c r="C2">
         <v>1</v>
       </c>
@@ -3515,20 +3702,17 @@
         <f>E2-F2</f>
         <v>55</v>
       </c>
-      <c r="H2" s="4">
-        <f>ROUND(F2*100/E2,6)</f>
-        <v>98.042704999999998</v>
-      </c>
-      <c r="I2" s="5">
-        <f>ROUND(AVERAGE(H2,H3),6)</f>
-        <v>98.256227999999993</v>
+      <c r="H2" s="10">
+        <v>0.98042704999999997</v>
+      </c>
+      <c r="I2" s="11">
+        <f>ROUND(AVERAGE(H2,H3),8)</f>
+        <v>0.98256228000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3545,17 +3729,16 @@
         <f t="shared" ref="G3:G35" si="0">E3-F3</f>
         <v>43</v>
       </c>
-      <c r="H3" s="4">
-        <f>ROUND(F3*100/E3,6)</f>
-        <v>98.469751000000002</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="H3" s="10">
+        <v>0.98469751000000005</v>
+      </c>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
         <v>15</v>
       </c>
       <c r="C4">
@@ -3574,20 +3757,17 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="H4" s="4">
-        <f>ROUND(F4*100/E4,6)</f>
-        <v>97.330961000000002</v>
-      </c>
-      <c r="I4" s="5">
-        <f>ROUND(AVERAGE(H4,H5),6)</f>
-        <v>97.437723000000005</v>
+      <c r="H4" s="10">
+        <v>0.97330961000000005</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" ref="I4" si="1">ROUND(AVERAGE(H4,H5),8)</f>
+        <v>0.97437722999999998</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -3604,17 +3784,16 @@
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="H5" s="4">
-        <f>ROUND(F5*100/E5,6)</f>
-        <v>97.544483999999997</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="H5" s="10">
+        <v>0.97544483999999998</v>
+      </c>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7">
         <v>14</v>
       </c>
       <c r="C6">
@@ -3633,20 +3812,17 @@
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="H6" s="4">
-        <f>ROUND(F6*100/E6,6)</f>
-        <v>97.295373999999995</v>
-      </c>
-      <c r="I6" s="5">
-        <f>ROUND(AVERAGE(H6,H7),6)</f>
-        <v>97.437723000000005</v>
+      <c r="H6" s="10">
+        <v>0.97295374000000001</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" ref="I6" si="2">ROUND(AVERAGE(H6,H7),8)</f>
+        <v>0.97437722999999998</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7">
         <v>2</v>
       </c>
@@ -3663,17 +3839,16 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="H7" s="4">
-        <f>ROUND(F7*100/E7,6)</f>
-        <v>97.580071000000004</v>
-      </c>
-      <c r="I7" s="5"/>
+      <c r="H7" s="10">
+        <v>0.97580071000000002</v>
+      </c>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7">
         <v>13</v>
       </c>
       <c r="C8">
@@ -3692,20 +3867,17 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="H8" s="4">
-        <f>ROUND(F8*100/E8,6)</f>
-        <v>97.508897000000005</v>
-      </c>
-      <c r="I8" s="5">
-        <f>ROUND(AVERAGE(H8,H9),6)</f>
-        <v>97.633452000000005</v>
+      <c r="H8" s="10">
+        <v>0.97508897000000005</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" ref="I8" si="3">ROUND(AVERAGE(H8,H9),8)</f>
+        <v>0.97633451999999998</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9">
         <v>2</v>
       </c>
@@ -3722,17 +3894,16 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H9" s="4">
-        <f>ROUND(F9*100/E9,6)</f>
-        <v>97.758007000000006</v>
-      </c>
-      <c r="I9" s="5"/>
+      <c r="H9" s="10">
+        <v>0.97758007000000013</v>
+      </c>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="A10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
         <v>12</v>
       </c>
       <c r="C10">
@@ -3751,20 +3922,17 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="H10" s="4">
-        <f>ROUND(F10*100/E10,6)</f>
-        <v>97.259786000000005</v>
-      </c>
-      <c r="I10" s="5">
-        <f>ROUND(AVERAGE(H10,H11),6)</f>
-        <v>97.544483999999997</v>
+      <c r="H10" s="10">
+        <v>0.97259786000000004</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" ref="I10" si="4">ROUND(AVERAGE(H10,H11),8)</f>
+        <v>0.97544483999999998</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11">
         <v>2</v>
       </c>
@@ -3781,17 +3949,16 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="H11" s="4">
-        <f>ROUND(F11*100/E11,6)</f>
-        <v>97.829181000000005</v>
-      </c>
-      <c r="I11" s="5"/>
+      <c r="H11" s="10">
+        <v>0.97829181000000009</v>
+      </c>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
         <v>11</v>
       </c>
       <c r="C12">
@@ -3810,20 +3977,17 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="H12" s="4">
-        <f>ROUND(F12*100/E12,6)</f>
-        <v>97.508897000000005</v>
-      </c>
-      <c r="I12" s="5">
-        <f>ROUND(AVERAGE(H12,H13),6)</f>
-        <v>97.633452000000005</v>
+      <c r="H12" s="10">
+        <v>0.97508897000000005</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" ref="I12" si="5">ROUND(AVERAGE(H12,H13),8)</f>
+        <v>0.97633451999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13">
         <v>2</v>
       </c>
@@ -3840,17 +4004,16 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H13" s="4">
-        <f>ROUND(F13*100/E13,6)</f>
-        <v>97.758007000000006</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="H13" s="10">
+        <v>0.97758007000000013</v>
+      </c>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7">
         <v>10</v>
       </c>
       <c r="C14">
@@ -3869,20 +4032,17 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="H14" s="4">
-        <f>ROUND(F14*100/E14,6)</f>
-        <v>97.615657999999996</v>
-      </c>
-      <c r="I14" s="5">
-        <f>ROUND(AVERAGE(H14,H15),6)</f>
-        <v>97.758007000000006</v>
+      <c r="H14" s="10">
+        <v>0.97615657999999994</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" ref="I14" si="6">ROUND(AVERAGE(H14,H15),8)</f>
+        <v>0.97758007000000002</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15">
         <v>2</v>
       </c>
@@ -3899,17 +4059,16 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H15" s="4">
-        <f>ROUND(F15*100/E15,6)</f>
-        <v>97.900356000000002</v>
-      </c>
-      <c r="I15" s="5"/>
+      <c r="H15" s="10">
+        <v>0.97900355999999999</v>
+      </c>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
         <v>9</v>
       </c>
       <c r="C16">
@@ -3928,20 +4087,17 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="H16" s="4">
-        <f t="shared" ref="H16:H35" si="1">ROUND(F16*100/E16,6)</f>
-        <v>97.935942999999995</v>
-      </c>
-      <c r="I16" s="5">
-        <f>ROUND(AVERAGE(H16,H17),6)</f>
-        <v>97.971530000000001</v>
+      <c r="H16" s="10">
+        <v>0.97935942999999992</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" ref="I16" si="7">ROUND(AVERAGE(H16,H17),8)</f>
+        <v>0.97971529999999996</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17">
         <v>2</v>
       </c>
@@ -3958,17 +4114,16 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>98.007116999999994</v>
-      </c>
-      <c r="I17" s="5"/>
+      <c r="H17" s="10">
+        <v>0.98007116999999999</v>
+      </c>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7">
         <v>8</v>
       </c>
       <c r="C18">
@@ -3987,20 +4142,17 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="H18" s="4">
-        <f t="shared" si="1"/>
-        <v>97.72242</v>
-      </c>
-      <c r="I18" s="5">
-        <f>ROUND(AVERAGE(H18,H19),6)</f>
-        <v>97.846975</v>
+      <c r="H18" s="10">
+        <v>0.97722419999999999</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" ref="I18" si="8">ROUND(AVERAGE(H18,H19),8)</f>
+        <v>0.97846975000000003</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="3"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19">
         <v>2</v>
       </c>
@@ -4017,17 +4169,16 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>97.971530000000001</v>
-      </c>
-      <c r="I19" s="5"/>
+      <c r="H19" s="10">
+        <v>0.97971530000000007</v>
+      </c>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="3">
+      <c r="A20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="7">
         <v>7</v>
       </c>
       <c r="C20">
@@ -4046,20 +4197,17 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>97.900356000000002</v>
-      </c>
-      <c r="I20" s="5">
-        <f>ROUND(AVERAGE(H20,H21),6)</f>
-        <v>97.971530999999999</v>
+      <c r="H20" s="10">
+        <v>0.97900355999999999</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" ref="I20" si="9">ROUND(AVERAGE(H20,H21),8)</f>
+        <v>0.97971531000000001</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="3"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
       <c r="C21">
         <v>2</v>
       </c>
@@ -4076,17 +4224,16 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H21" s="4">
-        <f t="shared" si="1"/>
-        <v>98.042704999999998</v>
-      </c>
-      <c r="I21" s="5"/>
+      <c r="H21" s="10">
+        <v>0.98042704999999997</v>
+      </c>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3">
+      <c r="A22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="7">
         <v>6</v>
       </c>
       <c r="C22">
@@ -4105,20 +4252,17 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>97.686832999999993</v>
-      </c>
-      <c r="I22" s="5">
-        <f>ROUND(AVERAGE(H22,H23),6)</f>
-        <v>97.900356000000002</v>
+      <c r="H22" s="10">
+        <v>0.97686832999999995</v>
+      </c>
+      <c r="I22" s="11">
+        <f t="shared" ref="I22" si="10">ROUND(AVERAGE(H22,H23),8)</f>
+        <v>0.97900355999999999</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
       <c r="C23">
         <v>2</v>
       </c>
@@ -4135,17 +4279,16 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>98.113878999999997</v>
-      </c>
-      <c r="I23" s="5"/>
+      <c r="H23" s="10">
+        <v>0.98113879000000004</v>
+      </c>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="3">
+      <c r="A24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="7">
         <v>5</v>
       </c>
       <c r="C24">
@@ -4164,20 +4307,17 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H24" s="4">
-        <f t="shared" si="1"/>
-        <v>97.758007000000006</v>
-      </c>
-      <c r="I24" s="5">
-        <f>ROUND(AVERAGE(H24,H25),6)</f>
-        <v>98.060497999999995</v>
+      <c r="H24" s="10">
+        <v>0.97758007000000013</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" ref="I24" si="11">ROUND(AVERAGE(H24,H25),8)</f>
+        <v>0.98060497999999996</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="3"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
       <c r="C25">
         <v>2</v>
       </c>
@@ -4194,17 +4334,16 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>98.362988999999999</v>
-      </c>
-      <c r="I25" s="5"/>
+      <c r="H25" s="10">
+        <v>0.98362989000000001</v>
+      </c>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="A26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="7">
         <v>4</v>
       </c>
       <c r="C26">
@@ -4223,20 +4362,17 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>97.864768999999995</v>
-      </c>
-      <c r="I26" s="5">
-        <f>ROUND(AVERAGE(H26,H27),6)</f>
-        <v>97.953737000000004</v>
+      <c r="H26" s="10">
+        <v>0.97864768999999996</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" ref="I26" si="12">ROUND(AVERAGE(H26,H27),8)</f>
+        <v>0.97953736999999996</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="3"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
       <c r="C27">
         <v>2</v>
       </c>
@@ -4253,17 +4389,16 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H27" s="4">
-        <f t="shared" si="1"/>
-        <v>98.042704999999998</v>
-      </c>
-      <c r="I27" s="5"/>
+      <c r="H27" s="10">
+        <v>0.98042704999999997</v>
+      </c>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="7">
         <v>3</v>
       </c>
       <c r="C28">
@@ -4282,20 +4417,17 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="H28" s="4">
-        <f t="shared" si="1"/>
-        <v>98.078292000000005</v>
-      </c>
-      <c r="I28" s="5">
-        <f>ROUND(AVERAGE(H28,H29),6)</f>
-        <v>98.096086</v>
+      <c r="H28" s="10">
+        <v>0.98078292000000011</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" ref="I28" si="13">ROUND(AVERAGE(H28,H29),8)</f>
+        <v>0.98096086000000005</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="3"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
       <c r="C29">
         <v>2</v>
       </c>
@@ -4312,17 +4444,16 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H29" s="4">
-        <f t="shared" si="1"/>
-        <v>98.113878999999997</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="H29" s="10">
+        <v>0.98113879000000004</v>
+      </c>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="3">
+      <c r="A30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="7">
         <v>2</v>
       </c>
       <c r="C30">
@@ -4341,20 +4472,17 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="H30" s="4">
-        <f t="shared" si="1"/>
-        <v>97.010676000000004</v>
-      </c>
-      <c r="I30" s="5">
-        <f>ROUND(AVERAGE(H30,H31),6)</f>
-        <v>97.330961000000002</v>
+      <c r="H30" s="10">
+        <v>0.97010676000000007</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" ref="I30" si="14">ROUND(AVERAGE(H30,H31),8)</f>
+        <v>0.97330961000000005</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="3"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
       <c r="C31">
         <v>2</v>
       </c>
@@ -4371,17 +4499,16 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="H31" s="4">
-        <f t="shared" si="1"/>
-        <v>97.651246</v>
-      </c>
-      <c r="I31" s="5"/>
+      <c r="H31" s="10">
+        <v>0.97651246000000003</v>
+      </c>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="3">
+      <c r="A32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="7">
         <v>1</v>
       </c>
       <c r="C32">
@@ -4400,20 +4527,17 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H32" s="4">
-        <f t="shared" si="1"/>
-        <v>98.042704999999998</v>
-      </c>
-      <c r="I32" s="5">
-        <f>ROUND(AVERAGE(H32,H33),6)</f>
-        <v>98.256227999999993</v>
+      <c r="H32" s="10">
+        <v>0.98042704999999997</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" ref="I32" si="15">ROUND(AVERAGE(H32,H33),8)</f>
+        <v>0.98256228000000001</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="3"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
       <c r="C33">
         <v>2</v>
       </c>
@@ -4430,17 +4554,16 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="H33" s="4">
-        <f t="shared" si="1"/>
-        <v>98.469751000000002</v>
-      </c>
-      <c r="I33" s="5"/>
+      <c r="H33" s="10">
+        <v>0.98469751000000005</v>
+      </c>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="6"/>
+      <c r="A34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="8"/>
       <c r="C34">
         <v>1</v>
       </c>
@@ -4457,20 +4580,17 @@
         <f t="shared" si="0"/>
         <v>284</v>
       </c>
-      <c r="H34" s="4">
-        <f t="shared" si="1"/>
-        <v>89.893237999999997</v>
-      </c>
-      <c r="I34" s="5">
-        <f>ROUND(AVERAGE(H34,H35),6)</f>
-        <v>90.427046000000004</v>
+      <c r="H34" s="10">
+        <v>0.89893237999999998</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" ref="I34" si="16">ROUND(AVERAGE(H34,H35),8)</f>
+        <v>0.90427046</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="6"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
       <c r="C35">
         <v>2</v>
       </c>
@@ -4487,35 +4607,142 @@
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="H35" s="4">
-        <f t="shared" si="1"/>
-        <v>90.960853999999998</v>
-      </c>
-      <c r="I35" s="5"/>
+      <c r="H35" s="10">
+        <v>0.90960854000000002</v>
+      </c>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>2810</v>
+      </c>
+      <c r="F36">
+        <v>1066</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ref="G36:G39" si="17">E36-F36</f>
+        <v>1744</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0.37935943000000005</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" ref="I36" si="18">ROUND(AVERAGE(H36,H37),8)</f>
+        <v>0.39003558999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>2810</v>
+      </c>
+      <c r="F37">
+        <v>1126</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="17"/>
+        <v>1684</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0.40071173999999998</v>
+      </c>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>2810</v>
+      </c>
+      <c r="F38">
+        <v>2508</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="17"/>
+        <v>302</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0.89252668999999996</v>
+      </c>
+      <c r="I38" s="11">
+        <f t="shared" ref="I38" si="19">ROUND(AVERAGE(H38,H39),8)</f>
+        <v>0.89697508999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>2810</v>
+      </c>
+      <c r="F39">
+        <v>2533</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="17"/>
+        <v>277</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0.90142348999999999</v>
+      </c>
+      <c r="I39" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="I28:I29"/>
+  <mergeCells count="57">
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I5"/>
@@ -4529,6 +4756,27 @@
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="I22:I23"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I28:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4539,13 +4787,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80050CAB-03EC-8548-BBAA-F2E0D74C6B64}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
@@ -4560,249 +4808,293 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="7">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3">
         <v>98.256227999999993</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="10">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
         <f>98.256228*0.01</f>
         <v>0.9825622799999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>97.437723000000005</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="10">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5">
         <f>98.096086*0.01</f>
         <v>0.98096086000000005</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>14</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="3">
         <v>97.437723000000005</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="10">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5">
         <f>90.427046*0.01</f>
         <v>0.90427046000000011</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>13</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>97.633452000000005</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10">
+        <f>39.003559*0.01</f>
+        <v>0.39003559000000004</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="3">
         <v>97.544483999999997</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10">
+        <f>89.697509*0.01</f>
+        <v>0.89697508999999997</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>11</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="3">
         <v>97.633452000000005</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>10</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="3">
         <v>97.758007000000006</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="10">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>97.971530000000001</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>97.846975</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
         <f>98.256228*0.01</f>
         <v>0.9825622799999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7">
-        <v>97.971530000000001</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="10">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>97.971530999999999</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5">
         <f>AVERAGE(C3:C17)*0.01</f>
         <v>0.97788849533333355</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>97.900356000000002</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7">
-        <v>97.846975</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="F12" s="5">
         <f>90.427046*0.01</f>
         <v>0.90427046000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7">
-        <v>97.971530999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7">
-        <v>97.900356000000002</v>
-      </c>
-    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="3">
         <v>98.060497999999995</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="10">
+        <f>39.003559*0.01</f>
+        <v>0.39003559000000004</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="3">
         <v>97.953737000000004</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="10">
+        <f>89.697509*0.01</f>
+        <v>0.89697508999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <v>98.096086</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="3">
         <v>97.330961000000002</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="3">
         <v>98.256227999999993</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3">
+        <v>90.427046000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="7">
-        <v>90.427046000000004</v>
+      <c r="C19">
+        <v>39.003559000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>89.697508999999997</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B43" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C43" s="9"/>
     </row>
@@ -4814,171 +5106,171 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B45" s="2">
         <v>15</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="6">
         <v>0.97437723000000009</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B46" s="2">
         <v>14</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="6">
         <v>0.97437723000000009</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B47" s="2">
         <v>13</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="6">
         <v>0.97633452000000009</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B48" s="2">
         <v>12</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="6">
         <v>0.97544483999999998</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B49" s="2">
         <v>11</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="6">
         <v>0.97633452000000009</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B50" s="2">
         <v>10</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="6">
         <v>0.97758007000000013</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B51" s="2">
         <v>9</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="6">
         <v>0.97971530000000007</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B52" s="2">
         <v>8</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="6">
         <v>0.97846975000000003</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B53" s="2">
         <v>7</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="6">
         <v>0.97971531000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B54" s="2">
         <v>6</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="6">
         <v>0.97900355999999999</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2">
         <v>5</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="6">
         <v>0.98060497999999996</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B56" s="2">
         <v>4</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="6">
         <v>0.97953737000000007</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B57" s="2">
         <v>3</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="6">
         <v>0.98096086000000005</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B58" s="2">
         <v>2</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="6">
         <v>0.97330961000000005</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="6">
         <v>0.9825622799999999</v>
       </c>
     </row>
@@ -4988,7 +5280,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F9" formulaRange="1"/>
+    <ignoredError sqref="F11" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
20220222T104400 - Nearest Neighbour implemented and complete. K-Nearest Neighbour implemented and complete. K-Means (simplified) implemented and complete. K-Means2 implemented and complete. K-Medians implemented and complete. Dataset shuffling implemented and complete. Included logs and statistics issued from DB.
</commit_message>
<xml_diff>
--- a/logs/stats.xlsx
+++ b/logs/stats.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD128GB/Google Drive/Education/MDX BSc CS/Modules/7 - CST3170 - Artificial Intelligence/Courseworks/CW2/Test/logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.camilleri\IdeaProjects\Test\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF820873-DE44-B743-A54F-25608F529726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="-20360" windowWidth="29400" windowHeight="18340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="-20355" windowWidth="29400" windowHeight="18345"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Aggregated" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
   <si>
     <t>Algorithm</t>
   </si>
@@ -84,11 +83,20 @@
   <si>
     <t>Supervised K-Medians</t>
   </si>
+  <si>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>TFVersion</t>
+  </si>
+  <si>
+    <t>AlgoID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000000%"/>
@@ -162,21 +170,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -192,9 +200,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -250,7 +258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -312,7 +320,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-C853-F84E-A589-8F8FB20ED03E}"/>
               </c:ext>
@@ -354,7 +362,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-C853-F84E-A589-8F8FB20ED03E}"/>
               </c:ext>
@@ -373,7 +381,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-D38A-9E4D-9E93-3B16D157EAA1}"/>
               </c:ext>
@@ -478,7 +486,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-MT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -489,7 +497,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -555,7 +563,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D38A-9E4D-9E93-3B16D157EAA1}"/>
             </c:ext>
@@ -572,11 +580,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="307465983"/>
-        <c:axId val="204341855"/>
+        <c:axId val="2048855424"/>
+        <c:axId val="2048851616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="307465983"/>
+        <c:axId val="2048855424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,10 +621,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204341855"/>
+        <c:crossAx val="2048851616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204341855"/>
+        <c:axId val="2048851616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,10 +677,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307465983"/>
+        <c:crossAx val="2048855424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -710,7 +718,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-MT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -722,9 +730,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -780,7 +788,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -842,7 +850,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-8E1C-A440-AADF-23717A4C8749}"/>
               </c:ext>
@@ -884,7 +892,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-8E1C-A440-AADF-23717A4C8749}"/>
               </c:ext>
@@ -903,7 +911,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-4338-CD4E-845A-F0ED836BBF7E}"/>
               </c:ext>
@@ -1007,7 +1015,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-MT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -1018,7 +1026,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1084,7 +1092,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4338-CD4E-845A-F0ED836BBF7E}"/>
             </c:ext>
@@ -1101,11 +1109,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="307760879"/>
-        <c:axId val="307734463"/>
+        <c:axId val="2048856512"/>
+        <c:axId val="2048851072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="307760879"/>
+        <c:axId val="2048856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,10 +1150,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307734463"/>
+        <c:crossAx val="2048851072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1153,7 +1161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="307734463"/>
+        <c:axId val="2048851072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,10 +1206,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307760879"/>
+        <c:crossAx val="2048856512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1239,7 +1247,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-MT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1251,9 +1259,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1309,7 +1317,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1493,7 +1501,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6418-FC4D-8E5D-C8EB1EB6E4CD}"/>
             </c:ext>
@@ -1507,11 +1515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205164303"/>
-        <c:axId val="307272383"/>
+        <c:axId val="2048852160"/>
+        <c:axId val="2048849440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="205164303"/>
+        <c:axId val="2048852160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1576,7 +1584,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-MT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1611,16 +1619,16 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307272383"/>
+        <c:crossAx val="2048849440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="307272383"/>
+        <c:axId val="2048849440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,10 +1678,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205164303"/>
+        <c:crossAx val="2048852160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,7 +1719,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-MT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3279,7 +3287,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2148EFD1-D9C9-5349-9DA6-C366F78F086B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2148EFD1-D9C9-5349-9DA6-C366F78F086B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3315,7 +3323,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636A8F4A-45B0-5F40-87F5-6E1CB0D0BAE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{636A8F4A-45B0-5F40-87F5-6E1CB0D0BAE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3351,7 +3359,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC4AB49D-87E6-C147-A8F0-AC03F2A310C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC4AB49D-87E6-C147-A8F0-AC03F2A310C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3634,1138 +3642,1646 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M39" sqref="M1:M39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="str">
+        <f>"INSERT INTO dbo.tb_ds_stats (TestID, fk_algorithm, kValue, fk_TrainingDataset, fk_TestDataset, SuccessfulClassifications, TwoFoldVersion) VALUES "</f>
+        <v xml:space="preserve">INSERT INTO dbo.tb_ds_stats (TestID, fk_algorithm, kValue, fk_TrainingDataset, fk_TestDataset, SuccessfulClassifications, TwoFoldVersion) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2">
-        <v>1</v>
-      </c>
+      <c r="C2" s="9"/>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>2810</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2755</v>
       </c>
-      <c r="G2">
-        <f>E2-F2</f>
+      <c r="H2">
+        <f>F2-G2</f>
         <v>55</v>
       </c>
-      <c r="H2" s="10">
+      <c r="I2" s="7">
         <v>0.98042704999999997</v>
       </c>
-      <c r="I2" s="11">
-        <f>ROUND(AVERAGE(H2,H3),8)</f>
+      <c r="J2" s="10">
+        <f>ROUND(AVERAGE(I2,I3),8)</f>
         <v>0.98256228000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="str">
+        <f>"(" &amp; K2 &amp; ", " &amp; A2 &amp; ", " &amp; IF(ISNUMBER(C2),C2,0) &amp; ", " &amp; D2 &amp; ", " &amp; E2 &amp; ", " &amp; G2 &amp; ", " &amp; L2 &amp; ")"</f>
+        <v>(1, 2, 0, 1, 2, 2755, 1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="8"/>
-      <c r="C3">
-        <v>2</v>
-      </c>
+      <c r="C3" s="9"/>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>2810</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2767</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G35" si="0">E3-F3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H35" si="0">F3-G3</f>
         <v>43</v>
       </c>
-      <c r="H3" s="10">
+      <c r="I3" s="7">
         <v>0.98469751000000005</v>
       </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="str">
+        <f>"(" &amp; K3 &amp; ", " &amp; A3 &amp; ", " &amp; IF(ISNUMBER(C3),C3,0) &amp; ", " &amp; D3 &amp; ", " &amp; E3 &amp; ", " &amp; G3 &amp; ", " &amp; L3 &amp; ")"</f>
+        <v>(1, 2, 0, 2, 1, 2767, 2)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7">
+      <c r="C4" s="8">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <v>2810</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2735</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="7">
         <v>0.97330961000000005</v>
       </c>
-      <c r="I4" s="11">
-        <f t="shared" ref="I4" si="1">ROUND(AVERAGE(H4,H5),8)</f>
+      <c r="J4" s="10">
+        <f t="shared" ref="J4" si="1">ROUND(AVERAGE(I4,I5),8)</f>
         <v>0.97437722999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5">
-        <v>2</v>
-      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M39" si="2">"(" &amp; K4 &amp; ", " &amp; A4 &amp; ", " &amp; IF(ISNUMBER(C4),C4,0) &amp; ", " &amp; D4 &amp; ", " &amp; E4 &amp; ", " &amp; G4 &amp; ", " &amp; L4 &amp; ")"</f>
+        <v>(2, 3, 15, 1, 2, 2735, 1)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2810</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>2741</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="7">
         <v>0.97544483999999998</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="2"/>
+        <v>(2, 3, 0, 2, 1, 2741, 2)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7">
+      <c r="C6" s="8">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
         <v>2810</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2734</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="7">
         <v>0.97295374000000001</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" ref="I6" si="2">ROUND(AVERAGE(H6,H7),8)</f>
+      <c r="J6" s="10">
+        <f t="shared" ref="J6" si="3">ROUND(AVERAGE(I6,I7),8)</f>
         <v>0.97437722999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7">
-        <v>2</v>
-      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v>(3, 3, 14, 1, 2, 2734, 1)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>2810</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2742</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="7">
         <v>0.97580071000000002</v>
       </c>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="2"/>
+        <v>(3, 3, 0, 2, 1, 2742, 2)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7">
+      <c r="C8" s="8">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
         <v>2810</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2740</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="7">
         <v>0.97508897000000005</v>
       </c>
-      <c r="I8" s="11">
-        <f t="shared" ref="I8" si="3">ROUND(AVERAGE(H8,H9),8)</f>
+      <c r="J8" s="10">
+        <f t="shared" ref="J8" si="4">ROUND(AVERAGE(I8,I9),8)</f>
         <v>0.97633451999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9">
-        <v>2</v>
-      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="2"/>
+        <v>(4, 3, 13, 1, 2, 2740, 1)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>2810</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2747</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="7">
         <v>0.97758007000000013</v>
       </c>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="J9" s="10"/>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="2"/>
+        <v>(4, 3, 0, 2, 1, 2747, 2)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7">
+      <c r="C10" s="8">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
         <v>2810</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2733</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="7">
         <v>0.97259786000000004</v>
       </c>
-      <c r="I10" s="11">
-        <f t="shared" ref="I10" si="4">ROUND(AVERAGE(H10,H11),8)</f>
+      <c r="J10" s="10">
+        <f t="shared" ref="J10" si="5">ROUND(AVERAGE(I10,I11),8)</f>
         <v>0.97544483999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11">
-        <v>2</v>
-      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 3, 12, 1, 2, 2733, 1)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>2810</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2749</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="H11" s="10">
+      <c r="I11" s="7">
         <v>0.97829181000000009</v>
       </c>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="J11" s="10"/>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 3, 0, 2, 1, 2749, 2)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="C12" s="8">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
         <v>2810</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2740</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="H12" s="10">
+      <c r="I12" s="7">
         <v>0.97508897000000005</v>
       </c>
-      <c r="I12" s="11">
-        <f t="shared" ref="I12" si="5">ROUND(AVERAGE(H12,H13),8)</f>
+      <c r="J12" s="10">
+        <f t="shared" ref="J12" si="6">ROUND(AVERAGE(I12,I13),8)</f>
         <v>0.97633451999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13">
-        <v>2</v>
-      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 3, 11, 1, 2, 2740, 1)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>2810</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>2747</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H13" s="10">
+      <c r="I13" s="7">
         <v>0.97758007000000013</v>
       </c>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="J13" s="10"/>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 3, 0, 2, 1, 2747, 2)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7">
+      <c r="C14" s="8">
         <v>10</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
         <v>2810</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>2743</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="H14" s="10">
+      <c r="I14" s="7">
         <v>0.97615657999999994</v>
       </c>
-      <c r="I14" s="11">
-        <f t="shared" ref="I14" si="6">ROUND(AVERAGE(H14,H15),8)</f>
+      <c r="J14" s="10">
+        <f t="shared" ref="J14" si="7">ROUND(AVERAGE(I14,I15),8)</f>
         <v>0.97758007000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15">
-        <v>2</v>
-      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="2"/>
+        <v>(7, 3, 10, 1, 2, 2743, 1)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>2810</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2751</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I15" s="7">
         <v>0.97900355999999999</v>
       </c>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="J15" s="10"/>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="2"/>
+        <v>(7, 3, 0, 2, 1, 2751, 2)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="7">
+      <c r="C16" s="8">
         <v>9</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
         <v>2810</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2752</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="H16" s="10">
+      <c r="I16" s="7">
         <v>0.97935942999999992</v>
       </c>
-      <c r="I16" s="11">
-        <f t="shared" ref="I16" si="7">ROUND(AVERAGE(H16,H17),8)</f>
+      <c r="J16" s="10">
+        <f t="shared" ref="J16" si="8">ROUND(AVERAGE(I16,I17),8)</f>
         <v>0.97971529999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17">
-        <v>2</v>
-      </c>
+      <c r="K16">
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="2"/>
+        <v>(8, 3, 9, 1, 2, 2752, 1)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>2810</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>2754</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="H17" s="10">
+      <c r="I17" s="7">
         <v>0.98007116999999999</v>
       </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17">
+        <v>8</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="2"/>
+        <v>(8, 3, 0, 2, 1, 2754, 2)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="7">
+      <c r="C18" s="8">
         <v>8</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
         <v>2810</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>2746</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I18" s="7">
         <v>0.97722419999999999</v>
       </c>
-      <c r="I18" s="11">
-        <f t="shared" ref="I18" si="8">ROUND(AVERAGE(H18,H19),8)</f>
+      <c r="J18" s="10">
+        <f t="shared" ref="J18" si="9">ROUND(AVERAGE(I18,I19),8)</f>
         <v>0.97846975000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19">
-        <v>2</v>
-      </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 3, 8, 1, 2, 2746, 1)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>2810</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>2753</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="H19" s="10">
+      <c r="I19" s="7">
         <v>0.97971530000000007</v>
       </c>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19">
+        <v>9</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 3, 0, 2, 1, 2753, 2)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="7">
+      <c r="C20" s="8">
         <v>7</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
         <v>2810</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>2751</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H20" s="10">
+      <c r="I20" s="7">
         <v>0.97900355999999999</v>
       </c>
-      <c r="I20" s="11">
-        <f t="shared" ref="I20" si="9">ROUND(AVERAGE(H20,H21),8)</f>
+      <c r="J20" s="10">
+        <f t="shared" ref="J20" si="10">ROUND(AVERAGE(I20,I21),8)</f>
         <v>0.97971531000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21">
-        <v>2</v>
-      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v>(10, 3, 7, 1, 2, 2751, 1)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>2810</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>2755</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H21" s="10">
+      <c r="I21" s="7">
         <v>0.98042704999999997</v>
       </c>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21">
         <v>10</v>
       </c>
-      <c r="B22" s="7">
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v>(10, 3, 0, 2, 1, 2755, 2)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="8">
         <v>6</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
         <v>2810</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>2745</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="H22" s="10">
+      <c r="I22" s="7">
         <v>0.97686832999999995</v>
       </c>
-      <c r="I22" s="11">
-        <f t="shared" ref="I22" si="10">ROUND(AVERAGE(H22,H23),8)</f>
+      <c r="J22" s="10">
+        <f t="shared" ref="J22" si="11">ROUND(AVERAGE(I22,I23),8)</f>
         <v>0.97900355999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23">
-        <v>2</v>
-      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v>(11, 3, 6, 1, 2, 2745, 1)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>2810</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>2757</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H23" s="10">
+      <c r="I23" s="7">
         <v>0.98113879000000004</v>
       </c>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23">
+        <v>11</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="2"/>
+        <v>(11, 3, 0, 2, 1, 2757, 2)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="7">
+      <c r="C24" s="8">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
         <v>2810</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>2747</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H24" s="10">
+      <c r="I24" s="7">
         <v>0.97758007000000013</v>
       </c>
-      <c r="I24" s="11">
-        <f t="shared" ref="I24" si="11">ROUND(AVERAGE(H24,H25),8)</f>
+      <c r="J24" s="10">
+        <f t="shared" ref="J24" si="12">ROUND(AVERAGE(I24,I25),8)</f>
         <v>0.98060497999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25">
-        <v>2</v>
-      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="2"/>
+        <v>(12, 3, 5, 1, 2, 2747, 1)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>2810</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>2764</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="H25" s="10">
+      <c r="I25" s="7">
         <v>0.98362989000000001</v>
       </c>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="J25" s="10"/>
+      <c r="K25">
+        <v>12</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="2"/>
+        <v>(12, 3, 0, 2, 1, 2764, 2)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="7">
+      <c r="C26" s="8">
         <v>4</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
         <v>2810</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>2750</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H26" s="10">
+      <c r="I26" s="7">
         <v>0.97864768999999996</v>
       </c>
-      <c r="I26" s="11">
-        <f t="shared" ref="I26" si="12">ROUND(AVERAGE(H26,H27),8)</f>
+      <c r="J26" s="10">
+        <f t="shared" ref="J26" si="13">ROUND(AVERAGE(I26,I27),8)</f>
         <v>0.97953736999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27">
-        <v>2</v>
-      </c>
+      <c r="K26">
+        <v>13</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="2"/>
+        <v>(13, 3, 4, 1, 2, 2750, 1)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
         <v>2810</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>2755</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H27" s="10">
+      <c r="I27" s="7">
         <v>0.98042704999999997</v>
       </c>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="J27" s="10"/>
+      <c r="K27">
+        <v>13</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="2"/>
+        <v>(13, 3, 0, 2, 1, 2755, 2)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="7">
+      <c r="C28" s="8">
         <v>3</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
         <v>2810</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>2756</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="H28" s="10">
+      <c r="I28" s="7">
         <v>0.98078292000000011</v>
       </c>
-      <c r="I28" s="11">
-        <f t="shared" ref="I28" si="13">ROUND(AVERAGE(H28,H29),8)</f>
+      <c r="J28" s="10">
+        <f t="shared" ref="J28" si="14">ROUND(AVERAGE(I28,I29),8)</f>
         <v>0.98096086000000005</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29">
-        <v>2</v>
-      </c>
+      <c r="K28">
+        <v>14</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="2"/>
+        <v>(14, 3, 3, 1, 2, 2756, 1)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>2810</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>2757</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I29" s="7">
         <v>0.98113879000000004</v>
       </c>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="J29" s="10"/>
+      <c r="K29">
+        <v>14</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v>(14, 3, 0, 2, 1, 2757, 2)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="7">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" s="8">
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
         <v>2810</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>2726</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="H30" s="10">
+      <c r="I30" s="7">
         <v>0.97010676000000007</v>
       </c>
-      <c r="I30" s="11">
-        <f t="shared" ref="I30" si="14">ROUND(AVERAGE(H30,H31),8)</f>
+      <c r="J30" s="10">
+        <f t="shared" ref="J30" si="15">ROUND(AVERAGE(I30,I31),8)</f>
         <v>0.97330961000000005</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31">
-        <v>2</v>
-      </c>
+      <c r="K30">
+        <v>15</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="2"/>
+        <v>(15, 3, 2, 1, 2, 2726, 1)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>2810</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>2744</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="H31" s="10">
+      <c r="I31" s="7">
         <v>0.97651246000000003</v>
       </c>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="J31" s="10"/>
+      <c r="K31">
+        <v>15</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="2"/>
+        <v>(15, 3, 0, 2, 1, 2744, 2)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32">
+      <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
         <v>2810</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>2755</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H32" s="10">
+      <c r="I32" s="7">
         <v>0.98042704999999997</v>
       </c>
-      <c r="I32" s="11">
-        <f t="shared" ref="I32" si="15">ROUND(AVERAGE(H32,H33),8)</f>
+      <c r="J32" s="10">
+        <f t="shared" ref="J32" si="16">ROUND(AVERAGE(I32,I33),8)</f>
         <v>0.98256228000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33">
-        <v>2</v>
-      </c>
+      <c r="K32">
+        <v>16</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="2"/>
+        <v>(16, 3, 1, 1, 2, 2755, 1)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>2810</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>2767</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="H33" s="10">
+      <c r="I33" s="7">
         <v>0.98469751000000005</v>
       </c>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="J33" s="10"/>
+      <c r="K33">
+        <v>16</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="2"/>
+        <v>(16, 3, 0, 2, 1, 2767, 2)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34">
-        <v>1</v>
-      </c>
+      <c r="C34" s="9"/>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
         <v>2810</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>2526</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="0"/>
         <v>284</v>
       </c>
-      <c r="H34" s="10">
+      <c r="I34" s="7">
         <v>0.89893237999999998</v>
       </c>
-      <c r="I34" s="11">
-        <f t="shared" ref="I34" si="16">ROUND(AVERAGE(H34,H35),8)</f>
+      <c r="J34" s="10">
+        <f t="shared" ref="J34" si="17">ROUND(AVERAGE(I34,I35),8)</f>
         <v>0.90427046</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="K34">
+        <v>17</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="2"/>
+        <v>(17, 4, 0, 1, 2, 2526, 1)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
       <c r="B35" s="8"/>
-      <c r="C35">
-        <v>2</v>
-      </c>
+      <c r="C35" s="9"/>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>2810</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>2556</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="H35" s="10">
+      <c r="I35" s="7">
         <v>0.90960854000000002</v>
       </c>
-      <c r="I35" s="11"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="J35" s="10"/>
+      <c r="K35">
+        <v>17</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="2"/>
+        <v>(17, 4, 0, 2, 1, 2556, 2)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36">
-        <v>1</v>
-      </c>
+      <c r="C36" s="9"/>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
         <v>2810</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>1066</v>
       </c>
-      <c r="G36">
-        <f t="shared" ref="G36:G39" si="17">E36-F36</f>
+      <c r="H36">
+        <f t="shared" ref="H36:H39" si="18">F36-G36</f>
         <v>1744</v>
       </c>
-      <c r="H36" s="10">
+      <c r="I36" s="7">
         <v>0.37935943000000005</v>
       </c>
-      <c r="I36" s="11">
-        <f t="shared" ref="I36" si="18">ROUND(AVERAGE(H36,H37),8)</f>
+      <c r="J36" s="10">
+        <f t="shared" ref="J36" si="19">ROUND(AVERAGE(I36,I37),8)</f>
         <v>0.39003558999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="K36">
+        <v>18</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="2"/>
+        <v>(18, 5, 0, 1, 2, 1066, 1)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
       <c r="B37" s="8"/>
-      <c r="C37">
-        <v>2</v>
-      </c>
+      <c r="C37" s="9"/>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>2810</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>1126</v>
       </c>
-      <c r="G37">
-        <f t="shared" si="17"/>
+      <c r="H37">
+        <f t="shared" si="18"/>
         <v>1684</v>
       </c>
-      <c r="H37" s="10">
+      <c r="I37" s="7">
         <v>0.40071173999999998</v>
       </c>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="J37" s="10"/>
+      <c r="K37">
+        <v>18</v>
+      </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="2"/>
+        <v>(18, 5, 0, 2, 1, 1126, 2)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38">
-        <v>1</v>
-      </c>
+      <c r="C38" s="9"/>
       <c r="D38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
         <v>2810</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>2508</v>
       </c>
-      <c r="G38">
-        <f t="shared" si="17"/>
+      <c r="H38">
+        <f t="shared" si="18"/>
         <v>302</v>
       </c>
-      <c r="H38" s="10">
+      <c r="I38" s="7">
         <v>0.89252668999999996</v>
       </c>
-      <c r="I38" s="11">
-        <f t="shared" ref="I38" si="19">ROUND(AVERAGE(H38,H39),8)</f>
+      <c r="J38" s="10">
+        <f t="shared" ref="J38" si="20">ROUND(AVERAGE(I38,I39),8)</f>
         <v>0.89697508999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+      <c r="K38">
+        <v>19</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="2"/>
+        <v>(19, 6, 0, 1, 2, 2508, 1)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6</v>
+      </c>
       <c r="B39" s="8"/>
-      <c r="C39">
-        <v>2</v>
-      </c>
+      <c r="C39" s="9"/>
       <c r="D39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>2810</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>2533</v>
       </c>
-      <c r="G39">
-        <f t="shared" si="17"/>
+      <c r="H39">
+        <f t="shared" si="18"/>
         <v>277</v>
       </c>
-      <c r="H39" s="10">
+      <c r="I39" s="7">
         <v>0.90142348999999999</v>
       </c>
-      <c r="I39" s="11"/>
+      <c r="J39" s="10"/>
+      <c r="K39">
+        <v>19</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="2"/>
+        <v>(19, 6, 0, 2, 1, 2533, 2)</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="J38:J39"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I12:I13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
@@ -4773,10 +5289,13 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4784,23 +5303,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80050CAB-03EC-8548-BBAA-F2E0D74C6B64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4817,7 +5336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -4833,7 +5352,7 @@
         <v>0.9825622799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -4851,7 +5370,7 @@
         <v>0.98096086000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -4869,7 +5388,7 @@
         <v>0.90427046000000011</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4882,12 +5401,12 @@
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <f>39.003559*0.01</f>
         <v>0.39003559000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4900,12 +5419,12 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <f>89.697509*0.01</f>
         <v>0.89697508999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4916,7 +5435,7 @@
         <v>97.633452000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -4927,7 +5446,7 @@
         <v>97.758007000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -4944,7 +5463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -4962,7 +5481,7 @@
         <v>0.9825622799999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -4980,7 +5499,7 @@
         <v>0.97788849533333355</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -4998,7 +5517,7 @@
         <v>0.90427046000000011</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -5011,12 +5530,12 @@
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <f>39.003559*0.01</f>
         <v>0.39003559000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -5029,12 +5548,12 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <f>89.697509*0.01</f>
         <v>0.89697508999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -5045,7 +5564,7 @@
         <v>98.096086</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -5056,7 +5575,7 @@
         <v>97.330961000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -5067,7 +5586,7 @@
         <v>98.256227999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -5076,7 +5595,7 @@
         <v>90.427046000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -5084,7 +5603,7 @@
         <v>39.003559000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -5092,13 +5611,13 @@
         <v>89.697508999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="9" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="11"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -5109,7 +5628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -5120,7 +5639,7 @@
         <v>0.97437723000000009</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>10</v>
       </c>
@@ -5131,7 +5650,7 @@
         <v>0.97437723000000009</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -5142,7 +5661,7 @@
         <v>0.97633452000000009</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -5153,7 +5672,7 @@
         <v>0.97544483999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -5164,7 +5683,7 @@
         <v>0.97633452000000009</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -5175,7 +5694,7 @@
         <v>0.97758007000000013</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -5186,7 +5705,7 @@
         <v>0.97971530000000007</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>10</v>
       </c>
@@ -5197,7 +5716,7 @@
         <v>0.97846975000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -5208,7 +5727,7 @@
         <v>0.97971531000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>10</v>
       </c>
@@ -5219,7 +5738,7 @@
         <v>0.97900355999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>10</v>
       </c>
@@ -5230,7 +5749,7 @@
         <v>0.98060497999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>10</v>
       </c>
@@ -5241,7 +5760,7 @@
         <v>0.97953737000000007</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>10</v>
       </c>
@@ -5252,7 +5771,7 @@
         <v>0.98096086000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>10</v>
       </c>
@@ -5263,7 +5782,7 @@
         <v>0.97330961000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>